<commit_message>
Updated the files with only 3 players replaced
</commit_message>
<xml_diff>
--- a/Data/TOR_PlayerReplacement.xlsx
+++ b/Data/TOR_PlayerReplacement.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\McMaster\DAT205\Capstone\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DD15A9-9E0F-429C-8FBD-B401BF6973D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A1D9D9-2FD7-41F4-BAF3-C983DF543552}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{42968B75-5DCE-4E0E-9A9A-B8A53223C097}"/>
   </bookViews>
   <sheets>
     <sheet name="TOR" sheetId="1" r:id="rId1"/>
     <sheet name="Non-TOR" sheetId="4" r:id="rId2"/>
+    <sheet name="TOR_Initial" sheetId="5" r:id="rId3"/>
+    <sheet name="Non-TOR_Initial" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="38">
   <si>
     <t>PLAYER_ID</t>
   </si>
@@ -503,7 +505,7 @@
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,178 +858,8 @@
         <v>13.298704081225454</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1628449</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5">
-        <v>12.481956521739132</v>
-      </c>
-      <c r="D5">
-        <v>2.0869565217391304</v>
-      </c>
-      <c r="E5">
-        <v>4.4927536231884062</v>
-      </c>
-      <c r="F5">
-        <v>0.37192753623188396</v>
-      </c>
-      <c r="G5">
-        <v>0.57971014492753625</v>
-      </c>
-      <c r="H5">
-        <v>1.7826086956521738</v>
-      </c>
-      <c r="I5">
-        <v>0.20427536231884058</v>
-      </c>
-      <c r="J5">
-        <v>1.318840579710145</v>
-      </c>
-      <c r="K5">
-        <v>1.6956521739130435</v>
-      </c>
-      <c r="L5">
-        <v>0.38720289855072459</v>
-      </c>
-      <c r="M5">
-        <v>1.5942028985507246</v>
-      </c>
-      <c r="N5">
-        <v>2.5942028985507246</v>
-      </c>
-      <c r="O5">
-        <v>4.1884057971014492</v>
-      </c>
-      <c r="P5">
-        <v>0.39130434782608697</v>
-      </c>
-      <c r="Q5">
-        <v>0.42028985507246375</v>
-      </c>
-      <c r="R5">
-        <v>0.3188405797101449</v>
-      </c>
-      <c r="S5">
-        <v>0.91304347826086951</v>
-      </c>
-      <c r="T5">
-        <v>0.27536231884057971</v>
-      </c>
-      <c r="U5">
-        <v>1.7246376811594204</v>
-      </c>
-      <c r="V5">
-        <v>1.3913043478260869</v>
-      </c>
-      <c r="W5">
-        <v>6.0724637681159424</v>
-      </c>
-      <c r="X5">
-        <v>1.3478260869565217</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>5.8760082056350313</v>
-      </c>
-      <c r="AB5">
-        <v>17.426078158129052</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1626178</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6">
-        <v>17.854102564102558</v>
-      </c>
-      <c r="D6">
-        <v>2.4461538461538463</v>
-      </c>
-      <c r="E6">
-        <v>5.2153846153846155</v>
-      </c>
-      <c r="F6">
-        <v>0.3938615384615386</v>
-      </c>
-      <c r="G6">
-        <v>4.6153846153846156E-2</v>
-      </c>
-      <c r="H6">
-        <v>0.36923076923076925</v>
-      </c>
-      <c r="I6">
-        <v>2.3076923076923078E-2</v>
-      </c>
-      <c r="J6">
-        <v>1.7076923076923076</v>
-      </c>
-      <c r="K6">
-        <v>2.3230769230769233</v>
-      </c>
-      <c r="L6">
-        <v>0.50910769230769237</v>
-      </c>
-      <c r="M6">
-        <v>1.7692307692307692</v>
-      </c>
-      <c r="N6">
-        <v>2.7384615384615385</v>
-      </c>
-      <c r="O6">
-        <v>4.5076923076923077</v>
-      </c>
-      <c r="P6">
-        <v>1.676923076923077</v>
-      </c>
-      <c r="Q6">
-        <v>0.92307692307692313</v>
-      </c>
-      <c r="R6">
-        <v>0.7384615384615385</v>
-      </c>
-      <c r="S6">
-        <v>0.36923076923076925</v>
-      </c>
-      <c r="T6">
-        <v>0.41538461538461541</v>
-      </c>
-      <c r="U6">
-        <v>1.8461538461538463</v>
-      </c>
-      <c r="V6">
-        <v>2.0769230769230771</v>
-      </c>
-      <c r="W6">
-        <v>6.6461538461538465</v>
-      </c>
-      <c r="X6">
-        <v>1.3538461538461539</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>6.8461216287306979</v>
-      </c>
-      <c r="AB6">
-        <v>15.00868409105632</v>
-      </c>
-    </row>
+    <row r="5" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1035,10 +867,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427216FC-37D8-411D-BA13-86BA098230C8}">
-  <dimension ref="A1:AB6"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,6 +963,896 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1628378</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>34.146908602150518</v>
+      </c>
+      <c r="D2">
+        <v>8.383064516129032</v>
+      </c>
+      <c r="E2">
+        <v>19.137096774193548</v>
+      </c>
+      <c r="F2">
+        <v>0.43537903225806435</v>
+      </c>
+      <c r="G2">
+        <v>2.4879032258064515</v>
+      </c>
+      <c r="H2">
+        <v>6.971774193548387</v>
+      </c>
+      <c r="I2">
+        <v>0.34543548387096773</v>
+      </c>
+      <c r="J2">
+        <v>3.846774193548387</v>
+      </c>
+      <c r="K2">
+        <v>4.633064516129032</v>
+      </c>
+      <c r="L2">
+        <v>0.73257258064516151</v>
+      </c>
+      <c r="M2">
+        <v>0.75</v>
+      </c>
+      <c r="N2">
+        <v>3.4475806451612905</v>
+      </c>
+      <c r="O2">
+        <v>4.19758064516129</v>
+      </c>
+      <c r="P2">
+        <v>4.044354838709677</v>
+      </c>
+      <c r="Q2">
+        <v>2.818548387096774</v>
+      </c>
+      <c r="R2">
+        <v>1.310483870967742</v>
+      </c>
+      <c r="S2">
+        <v>0.31854838709677419</v>
+      </c>
+      <c r="T2">
+        <v>1.0806451612903225</v>
+      </c>
+      <c r="U2">
+        <v>2.6370967741935485</v>
+      </c>
+      <c r="V2">
+        <v>3.745967741935484</v>
+      </c>
+      <c r="W2">
+        <v>23.100806451612904</v>
+      </c>
+      <c r="X2">
+        <v>3.2983870967741935</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>16.026093974143031</v>
+      </c>
+      <c r="AB2">
+        <v>20.206097506408277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>204002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>0.75</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>6</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>3</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>6</v>
+      </c>
+      <c r="X3">
+        <v>4</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>17.054263565891471</v>
+      </c>
+      <c r="AB3">
+        <v>23.08133333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1628369</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>32.707450617283968</v>
+      </c>
+      <c r="D4">
+        <v>6.4148148148148145</v>
+      </c>
+      <c r="E4">
+        <v>14.088888888888889</v>
+      </c>
+      <c r="F4">
+        <v>0.45251111111111125</v>
+      </c>
+      <c r="G4">
+        <v>1.8148148148148149</v>
+      </c>
+      <c r="H4">
+        <v>4.6296296296296298</v>
+      </c>
+      <c r="I4">
+        <v>0.37565925925925936</v>
+      </c>
+      <c r="J4">
+        <v>3.2333333333333334</v>
+      </c>
+      <c r="K4">
+        <v>3.9185185185185185</v>
+      </c>
+      <c r="L4">
+        <v>0.66445925925925919</v>
+      </c>
+      <c r="M4">
+        <v>0.82592592592592595</v>
+      </c>
+      <c r="N4">
+        <v>5.2925925925925927</v>
+      </c>
+      <c r="O4">
+        <v>6.1185185185185187</v>
+      </c>
+      <c r="P4">
+        <v>2.4074074074074074</v>
+      </c>
+      <c r="Q4">
+        <v>1.8444444444444446</v>
+      </c>
+      <c r="R4">
+        <v>1.1481481481481481</v>
+      </c>
+      <c r="S4">
+        <v>0.77407407407407403</v>
+      </c>
+      <c r="T4">
+        <v>0.79629629629629628</v>
+      </c>
+      <c r="U4">
+        <v>2.1703703703703705</v>
+      </c>
+      <c r="V4">
+        <v>3.1</v>
+      </c>
+      <c r="W4">
+        <v>17.877777777777776</v>
+      </c>
+      <c r="X4">
+        <v>4.9592592592592597</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>15.703257802106853</v>
+      </c>
+      <c r="AB4">
+        <v>19.136810388531913</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B99B869-A144-4D80-983D-904FDA8447C7}">
+  <dimension ref="A1:AB6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AB6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1629044</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>2.645833333333333</v>
+      </c>
+      <c r="D2">
+        <v>0.75</v>
+      </c>
+      <c r="E2">
+        <v>1.25</v>
+      </c>
+      <c r="F2">
+        <v>0.41675000000000001</v>
+      </c>
+      <c r="G2">
+        <v>0.25</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.25</v>
+      </c>
+      <c r="J2">
+        <v>0.5</v>
+      </c>
+      <c r="K2">
+        <v>0.5</v>
+      </c>
+      <c r="L2">
+        <v>0.25</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0.25</v>
+      </c>
+      <c r="O2">
+        <v>0.25</v>
+      </c>
+      <c r="P2">
+        <v>0.5</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0.25</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0.5</v>
+      </c>
+      <c r="V2">
+        <v>0.25</v>
+      </c>
+      <c r="W2">
+        <v>2.25</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>1.778817664510995</v>
+      </c>
+      <c r="AB2">
+        <v>37.431452141608389</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1627775</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>24.54436936936937</v>
+      </c>
+      <c r="D3">
+        <v>1.8108108108108107</v>
+      </c>
+      <c r="E3">
+        <v>4.3783783783783781</v>
+      </c>
+      <c r="F3">
+        <v>0.3971351351351351</v>
+      </c>
+      <c r="G3">
+        <v>0.6216216216216216</v>
+      </c>
+      <c r="H3">
+        <v>1.9189189189189189</v>
+      </c>
+      <c r="I3">
+        <v>0.25494594594594594</v>
+      </c>
+      <c r="J3">
+        <v>0.35135135135135137</v>
+      </c>
+      <c r="K3">
+        <v>0.48648648648648651</v>
+      </c>
+      <c r="L3">
+        <v>0.1891891891891892</v>
+      </c>
+      <c r="M3">
+        <v>0.51351351351351349</v>
+      </c>
+      <c r="N3">
+        <v>1.8108108108108107</v>
+      </c>
+      <c r="O3">
+        <v>2.3243243243243241</v>
+      </c>
+      <c r="P3">
+        <v>2.1351351351351351</v>
+      </c>
+      <c r="Q3">
+        <v>0.78378378378378377</v>
+      </c>
+      <c r="R3">
+        <v>1.0540540540540539</v>
+      </c>
+      <c r="S3">
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="T3">
+        <v>0.21621621621621623</v>
+      </c>
+      <c r="U3">
+        <v>1.6216216216216217</v>
+      </c>
+      <c r="V3">
+        <v>0.40540540540540543</v>
+      </c>
+      <c r="W3">
+        <v>4.5945945945945947</v>
+      </c>
+      <c r="X3">
+        <v>5.4054054054054057E-2</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>4.3968925933061556</v>
+      </c>
+      <c r="AB3">
+        <v>7.6624284150229727</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1626169</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>6.0676190476190488</v>
+      </c>
+      <c r="D4">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="E4">
+        <v>2.5</v>
+      </c>
+      <c r="F4">
+        <v>0.24289285714285716</v>
+      </c>
+      <c r="G4">
+        <v>0.32142857142857145</v>
+      </c>
+      <c r="H4">
+        <v>1.0357142857142858</v>
+      </c>
+      <c r="I4">
+        <v>8.0357142857142863E-2</v>
+      </c>
+      <c r="J4">
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="K4">
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="L4">
+        <v>0.19046428571428572</v>
+      </c>
+      <c r="M4">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="N4">
+        <v>1.1785714285714286</v>
+      </c>
+      <c r="O4">
+        <v>1.4642857142857142</v>
+      </c>
+      <c r="P4">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="Q4">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="R4">
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="S4">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="T4">
+        <v>0.25</v>
+      </c>
+      <c r="U4">
+        <v>0.6785714285714286</v>
+      </c>
+      <c r="V4">
+        <v>0.39285714285714285</v>
+      </c>
+      <c r="W4">
+        <v>2.6071428571428572</v>
+      </c>
+      <c r="X4">
+        <v>0.25</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>1.8947842030763842</v>
+      </c>
+      <c r="AB4">
+        <v>13.298704081225454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1628449</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>12.481956521739132</v>
+      </c>
+      <c r="D5">
+        <v>2.0869565217391304</v>
+      </c>
+      <c r="E5">
+        <v>4.4927536231884062</v>
+      </c>
+      <c r="F5">
+        <v>0.37192753623188396</v>
+      </c>
+      <c r="G5">
+        <v>0.57971014492753625</v>
+      </c>
+      <c r="H5">
+        <v>1.7826086956521738</v>
+      </c>
+      <c r="I5">
+        <v>0.20427536231884058</v>
+      </c>
+      <c r="J5">
+        <v>1.318840579710145</v>
+      </c>
+      <c r="K5">
+        <v>1.6956521739130435</v>
+      </c>
+      <c r="L5">
+        <v>0.38720289855072459</v>
+      </c>
+      <c r="M5">
+        <v>1.5942028985507246</v>
+      </c>
+      <c r="N5">
+        <v>2.5942028985507246</v>
+      </c>
+      <c r="O5">
+        <v>4.1884057971014492</v>
+      </c>
+      <c r="P5">
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="Q5">
+        <v>0.42028985507246375</v>
+      </c>
+      <c r="R5">
+        <v>0.3188405797101449</v>
+      </c>
+      <c r="S5">
+        <v>0.91304347826086951</v>
+      </c>
+      <c r="T5">
+        <v>0.27536231884057971</v>
+      </c>
+      <c r="U5">
+        <v>1.7246376811594204</v>
+      </c>
+      <c r="V5">
+        <v>1.3913043478260869</v>
+      </c>
+      <c r="W5">
+        <v>6.0724637681159424</v>
+      </c>
+      <c r="X5">
+        <v>1.3478260869565217</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>5.8760082056350313</v>
+      </c>
+      <c r="AB5">
+        <v>17.426078158129052</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1626178</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>17.854102564102558</v>
+      </c>
+      <c r="D6">
+        <v>2.4461538461538463</v>
+      </c>
+      <c r="E6">
+        <v>5.2153846153846155</v>
+      </c>
+      <c r="F6">
+        <v>0.3938615384615386</v>
+      </c>
+      <c r="G6">
+        <v>4.6153846153846156E-2</v>
+      </c>
+      <c r="H6">
+        <v>0.36923076923076925</v>
+      </c>
+      <c r="I6">
+        <v>2.3076923076923078E-2</v>
+      </c>
+      <c r="J6">
+        <v>1.7076923076923076</v>
+      </c>
+      <c r="K6">
+        <v>2.3230769230769233</v>
+      </c>
+      <c r="L6">
+        <v>0.50910769230769237</v>
+      </c>
+      <c r="M6">
+        <v>1.7692307692307692</v>
+      </c>
+      <c r="N6">
+        <v>2.7384615384615385</v>
+      </c>
+      <c r="O6">
+        <v>4.5076923076923077</v>
+      </c>
+      <c r="P6">
+        <v>1.676923076923077</v>
+      </c>
+      <c r="Q6">
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="R6">
+        <v>0.7384615384615385</v>
+      </c>
+      <c r="S6">
+        <v>0.36923076923076925</v>
+      </c>
+      <c r="T6">
+        <v>0.41538461538461541</v>
+      </c>
+      <c r="U6">
+        <v>1.8461538461538463</v>
+      </c>
+      <c r="V6">
+        <v>2.0769230769230771</v>
+      </c>
+      <c r="W6">
+        <v>6.6461538461538465</v>
+      </c>
+      <c r="X6">
+        <v>1.3538461538461539</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>6.8461216287306979</v>
+      </c>
+      <c r="AB6">
+        <v>15.00868409105632</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F429CCD9-6B48-4B08-AB84-B5A604FBC773}">
+  <dimension ref="A1:AB6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AB6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1627732</v>
       </c>
       <c r="B2" t="s">

</xml_diff>